<commit_message>
PMO-2198: progress in working test cases, correction for loss carried forward and comparing incremental for commission
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/PMO-2198_a___SSC_usual.xlsx
+++ b/test/data/spreadsheets/PMO-2198_a___SSC_usual.xlsx
@@ -985,18 +985,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="#,##0;\-#,##0;"/>
     <numFmt numFmtId="169" formatCode="#,##0;\-#,##0;0"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0;\-#,##0.00;"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00;\-#,##0.00;0.00"/>
-    <numFmt numFmtId="174" formatCode="#,##0.000;\-#,##0.000;0.000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0;\-#,##0.00;"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00;\-#,##0.00;0.00"/>
+    <numFmt numFmtId="172" formatCode="#,##0.000;\-#,##0.000;0.000"/>
+    <numFmt numFmtId="187" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1107,8 +1108,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1171,6 +1179,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1417,14 +1430,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1787,26 +1801,35 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="14" fillId="10" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="15" fillId="11" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="14" fillId="10" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="15" fillId="11" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="14" fillId="10" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="3"/>
+    <xf numFmtId="9" fontId="14" fillId="10" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="16" fillId="12" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="14" fillId="10" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="14" fillId="10" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Dezimal 2" xfId="2"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1"/>
@@ -2473,25 +2496,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="53813632"/>
-        <c:axId val="53815168"/>
+        <c:axId val="52091520"/>
+        <c:axId val="53612928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53813632"/>
+        <c:axId val="52091520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53815168"/>
+        <c:crossAx val="53612928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53815168"/>
+        <c:axId val="53612928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2499,7 +2522,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53813632"/>
+        <c:crossAx val="52091520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2511,7 +2534,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2793,11 +2816,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="53832704"/>
-        <c:axId val="53757056"/>
+        <c:axId val="54863360"/>
+        <c:axId val="54870016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53832704"/>
+        <c:axId val="54863360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2822,13 +2845,13 @@
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53757056"/>
+        <c:crossAx val="54870016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53757056"/>
+        <c:axId val="54870016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2854,7 +2877,7 @@
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53832704"/>
+        <c:crossAx val="54863360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5475,10 +5498,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AY287"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3480" topLeftCell="A194" activePane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2784" topLeftCell="A185" activePane="bottomLeft"/>
       <selection activeCell="C215" sqref="C215"/>
-      <selection pane="bottomLeft" activeCell="C209" sqref="C209"/>
+      <selection pane="bottomLeft" activeCell="K191" sqref="K191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -5487,6 +5510,8 @@
     <col min="2" max="2" width="42.109375" style="122" customWidth="1"/>
     <col min="3" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="9" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5747,11 +5772,11 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" ht="14.4">
       <c r="B25" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="253">
         <v>0</v>
       </c>
       <c r="D25" s="41">
@@ -6063,14 +6088,14 @@
       <c r="W45" s="35"/>
       <c r="X45" s="35"/>
     </row>
-    <row r="46" spans="1:24">
+    <row r="46" spans="1:24" ht="14.4">
       <c r="A46" s="35"/>
       <c r="B46" s="35"/>
       <c r="C46" s="35"/>
-      <c r="D46" s="44">
-        <v>0</v>
-      </c>
-      <c r="E46" s="44">
+      <c r="D46" s="254">
+        <v>0</v>
+      </c>
+      <c r="E46" s="254">
         <v>0</v>
       </c>
       <c r="F46" s="35"/>
@@ -6135,14 +6160,14 @@
       <c r="W47" s="35"/>
       <c r="X47" s="35"/>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" ht="14.4">
       <c r="A48" s="35"/>
       <c r="B48" s="35"/>
       <c r="C48" s="35"/>
       <c r="D48" s="44">
         <v>0.5</v>
       </c>
-      <c r="E48" s="44">
+      <c r="E48" s="254">
         <v>0</v>
       </c>
       <c r="F48" s="35"/>
@@ -6171,12 +6196,12 @@
       <c r="W48" s="35"/>
       <c r="X48" s="35"/>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" ht="14.4">
       <c r="A49" s="35"/>
       <c r="B49" s="35"/>
       <c r="C49" s="35"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
+      <c r="D49" s="254"/>
+      <c r="E49" s="254"/>
       <c r="F49" s="35"/>
       <c r="G49" s="35"/>
       <c r="H49" s="27">
@@ -6551,7 +6576,7 @@
         <v>8.699999999999998E-2</v>
       </c>
       <c r="C63" s="192">
-        <f t="dataTable" ref="C63:F63" dt2D="0" dtr="1" r1="D57" ca="1"/>
+        <f t="dataTable" ref="C63:F63" dt2D="0" dtr="1" r1="D57"/>
         <v>4.349999999999999E-2</v>
       </c>
       <c r="D63" s="192">
@@ -6689,7 +6714,7 @@
         <v>8.699999999999998E-2</v>
       </c>
       <c r="C69" s="126">
-        <f t="dataTable" ref="C69:F69" dt2D="0" dtr="1" r1="D57"/>
+        <f t="dataTable" ref="C69:F69" dt2D="0" dtr="1" r1="D57" ca="1"/>
         <v>0</v>
       </c>
       <c r="D69" s="126">
@@ -7364,7 +7389,7 @@
         <v>0.17999999999999994</v>
       </c>
       <c r="J102" s="126">
-        <f t="dataTable" ref="J102:AY102" dt2D="0" dtr="1" r1="D105" ca="1"/>
+        <f t="dataTable" ref="J102:AY102" dt2D="0" dtr="1" r1="D105"/>
         <v>0.9</v>
       </c>
       <c r="K102" s="126">
@@ -7764,7 +7789,7 @@
         <v>0.17999999999999994</v>
       </c>
       <c r="C118" s="192">
-        <f t="dataTable" ref="C118:F118" dt2D="0" dtr="1" r1="D105"/>
+        <f t="dataTable" ref="C118:F118" dt2D="0" dtr="1" r1="D105" ca="1"/>
         <v>0.45284999999999997</v>
       </c>
       <c r="D118" s="192">
@@ -8328,19 +8353,19 @@
       <c r="B156" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="C156" s="159">
+      <c r="C156" s="258">
         <f t="shared" ref="C156:F159" si="23">C16*$C$22*(1-C78-$C$151-$C$152)</f>
         <v>61.830999999999989</v>
       </c>
-      <c r="D156" s="160">
+      <c r="D156" s="243">
         <f t="shared" si="23"/>
         <v>64.495500000000007</v>
       </c>
-      <c r="E156" s="160">
+      <c r="E156" s="243">
         <f t="shared" si="23"/>
         <v>67.344471000000013</v>
       </c>
-      <c r="F156" s="160">
+      <c r="F156" s="243">
         <f t="shared" si="23"/>
         <v>70.706996999999987</v>
       </c>
@@ -8352,19 +8377,19 @@
       <c r="B157" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="C157" s="158">
+      <c r="C157" s="243">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D157" s="161">
+      <c r="D157" s="244">
         <f t="shared" si="23"/>
         <v>64.495500000000007</v>
       </c>
-      <c r="E157" s="160">
+      <c r="E157" s="243">
         <f t="shared" si="23"/>
         <v>67.250519999999995</v>
       </c>
-      <c r="F157" s="160">
+      <c r="F157" s="243">
         <f t="shared" si="23"/>
         <v>68.333420249999989</v>
       </c>
@@ -8373,19 +8398,19 @@
       <c r="B158" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="C158" s="158">
+      <c r="C158" s="243">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D158" s="158">
+      <c r="D158" s="243">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="E158" s="161">
+      <c r="E158" s="244">
         <f t="shared" si="23"/>
         <v>47.690899999999999</v>
       </c>
-      <c r="F158" s="160">
+      <c r="F158" s="243">
         <f t="shared" si="23"/>
         <v>46.100594999999991</v>
       </c>
@@ -8394,19 +8419,19 @@
       <c r="B159" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="C159" s="158">
+      <c r="C159" s="243">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D159" s="158">
+      <c r="D159" s="243">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="E159" s="158">
+      <c r="E159" s="243">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="F159" s="161">
+      <c r="F159" s="244">
         <f t="shared" si="23"/>
         <v>26.352999999999998</v>
       </c>
@@ -8588,19 +8613,19 @@
       <c r="B174" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="C174" s="159">
+      <c r="C174" s="258">
         <f t="shared" ref="C174:F177" si="26">IF($C$171="yes",C166,C156)</f>
         <v>61.830999999999989</v>
       </c>
-      <c r="D174" s="160">
+      <c r="D174" s="243">
         <f t="shared" si="26"/>
         <v>64.495500000000007</v>
       </c>
-      <c r="E174" s="160">
+      <c r="E174" s="243">
         <f t="shared" si="26"/>
         <v>67.344471000000013</v>
       </c>
-      <c r="F174" s="160">
+      <c r="F174" s="243">
         <f t="shared" si="26"/>
         <v>70.706996999999987</v>
       </c>
@@ -8609,19 +8634,19 @@
       <c r="B175" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="C175" s="158">
+      <c r="C175" s="243">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="D175" s="161">
+      <c r="D175" s="244">
         <f t="shared" si="26"/>
         <v>64.495500000000007</v>
       </c>
-      <c r="E175" s="160">
+      <c r="E175" s="243">
         <f t="shared" si="26"/>
         <v>67.250519999999995</v>
       </c>
-      <c r="F175" s="160">
+      <c r="F175" s="243">
         <f t="shared" si="26"/>
         <v>68.333420249999989</v>
       </c>
@@ -8630,58 +8655,58 @@
       <c r="B176" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="C176" s="158">
+      <c r="C176" s="243">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="D176" s="158">
+      <c r="D176" s="243">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="E176" s="161">
+      <c r="E176" s="244">
         <f t="shared" si="26"/>
         <v>47.690899999999999</v>
       </c>
-      <c r="F176" s="160">
+      <c r="F176" s="243">
         <f t="shared" si="26"/>
         <v>46.100594999999991</v>
       </c>
     </row>
-    <row r="177" spans="2:8" outlineLevel="1">
+    <row r="177" spans="2:11" outlineLevel="1">
       <c r="B177" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="C177" s="158">
+      <c r="C177" s="243">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="D177" s="158">
+      <c r="D177" s="243">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="E177" s="158">
+      <c r="E177" s="243">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="F177" s="161">
+      <c r="F177" s="244">
         <f t="shared" si="26"/>
         <v>26.352999999999998</v>
       </c>
     </row>
-    <row r="178" spans="2:8" outlineLevel="1">
+    <row r="178" spans="2:11" outlineLevel="1">
       <c r="C178" s="158"/>
       <c r="D178" s="158"/>
       <c r="E178" s="158"/>
       <c r="F178" s="162"/>
     </row>
-    <row r="179" spans="2:8" outlineLevel="1">
+    <row r="179" spans="2:11" outlineLevel="1">
       <c r="B179" s="175"/>
       <c r="C179" s="201"/>
       <c r="D179" s="201"/>
       <c r="E179" s="201"/>
       <c r="F179" s="186"/>
     </row>
-    <row r="180" spans="2:8" ht="14.4" outlineLevel="1">
+    <row r="180" spans="2:11" ht="14.4" outlineLevel="1">
       <c r="B180" s="174" t="s">
         <v>237</v>
       </c>
@@ -8698,23 +8723,23 @@
         <v>113</v>
       </c>
     </row>
-    <row r="181" spans="2:8" outlineLevel="1">
+    <row r="181" spans="2:11" ht="14.4" outlineLevel="1">
       <c r="B181" s="175" t="s">
         <v>112</v>
       </c>
-      <c r="C181" s="199">
+      <c r="C181" s="257">
         <f>C16*$C$22* $C$151</f>
         <v>17.52</v>
       </c>
-      <c r="D181" s="200">
+      <c r="D181" s="250">
         <f t="shared" ref="D181:F181" si="27">D16*$C$22* $C$151</f>
         <v>18.395999999999997</v>
       </c>
-      <c r="E181" s="200">
+      <c r="E181" s="250">
         <f t="shared" si="27"/>
         <v>19.315799999999999</v>
       </c>
-      <c r="F181" s="200">
+      <c r="F181" s="250">
         <f t="shared" si="27"/>
         <v>20.281589999999998</v>
       </c>
@@ -8722,90 +8747,90 @@
         <v>238</v>
       </c>
     </row>
-    <row r="182" spans="2:8" outlineLevel="1">
+    <row r="182" spans="2:11" outlineLevel="1">
       <c r="B182" s="175" t="s">
         <v>111</v>
       </c>
-      <c r="C182" s="201">
+      <c r="C182" s="250">
         <f t="shared" ref="C182:F182" si="28">C17*$C$22* $C$151</f>
         <v>0</v>
       </c>
-      <c r="D182" s="202">
+      <c r="D182" s="252">
         <f t="shared" si="28"/>
         <v>18.395999999999997</v>
       </c>
-      <c r="E182" s="200">
+      <c r="E182" s="250">
         <f t="shared" si="28"/>
         <v>19.315799999999999</v>
       </c>
-      <c r="F182" s="200">
+      <c r="F182" s="250">
         <f t="shared" si="28"/>
         <v>20.281589999999998</v>
       </c>
     </row>
-    <row r="183" spans="2:8" outlineLevel="1">
+    <row r="183" spans="2:11" outlineLevel="1">
       <c r="B183" s="175" t="s">
         <v>110</v>
       </c>
-      <c r="C183" s="201">
+      <c r="C183" s="250">
         <f t="shared" ref="C183:F183" si="29">C18*$C$22* $C$151</f>
         <v>0</v>
       </c>
-      <c r="D183" s="201">
+      <c r="D183" s="250">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="E183" s="202">
+      <c r="E183" s="252">
         <f t="shared" si="29"/>
         <v>16.643999999999998</v>
       </c>
-      <c r="F183" s="200">
+      <c r="F183" s="250">
         <f t="shared" si="29"/>
         <v>17.476199999999999</v>
       </c>
     </row>
-    <row r="184" spans="2:8" outlineLevel="1">
+    <row r="184" spans="2:11" outlineLevel="1">
       <c r="B184" s="175" t="s">
         <v>109</v>
       </c>
-      <c r="C184" s="201">
+      <c r="C184" s="250">
         <f t="shared" ref="C184:F184" si="30">C19*$C$22* $C$151</f>
         <v>0</v>
       </c>
-      <c r="D184" s="201">
+      <c r="D184" s="250">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="E184" s="201">
+      <c r="E184" s="250">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="F184" s="202">
+      <c r="F184" s="252">
         <f t="shared" si="30"/>
         <v>14.891999999999999</v>
       </c>
     </row>
-    <row r="185" spans="2:8" outlineLevel="1">
+    <row r="185" spans="2:11" outlineLevel="1">
       <c r="C185" s="158"/>
       <c r="D185" s="158"/>
       <c r="E185" s="158"/>
       <c r="F185" s="162"/>
     </row>
-    <row r="186" spans="2:8" s="172" customFormat="1" outlineLevel="1">
+    <row r="186" spans="2:11" s="172" customFormat="1" outlineLevel="1">
       <c r="B186" s="175"/>
       <c r="C186" s="201"/>
       <c r="D186" s="201"/>
       <c r="E186" s="201"/>
       <c r="F186" s="186"/>
     </row>
-    <row r="187" spans="2:8" s="172" customFormat="1" outlineLevel="1">
+    <row r="187" spans="2:11" s="172" customFormat="1" outlineLevel="1">
       <c r="B187" s="175"/>
       <c r="C187" s="201"/>
       <c r="D187" s="201"/>
       <c r="E187" s="201"/>
       <c r="F187" s="186"/>
     </row>
-    <row r="188" spans="2:8" ht="14.4" outlineLevel="1">
+    <row r="188" spans="2:11" ht="14.4" outlineLevel="1">
       <c r="B188" s="123" t="s">
         <v>239</v>
       </c>
@@ -8825,88 +8850,139 @@
         <v>215</v>
       </c>
     </row>
-    <row r="189" spans="2:8" outlineLevel="1">
+    <row r="189" spans="2:11" outlineLevel="1">
       <c r="B189" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="C189" s="159">
+      <c r="C189" s="258">
         <f>$C$153*MAX(0,C174)</f>
         <v>40.808459999999997</v>
       </c>
-      <c r="D189" s="160">
+      <c r="D189" s="243">
         <f t="shared" ref="D189:F189" si="31">$C$153*MAX(0,D174)</f>
         <v>42.56703000000001</v>
       </c>
-      <c r="E189" s="160">
+      <c r="E189" s="243">
         <f t="shared" si="31"/>
         <v>44.447350860000007</v>
       </c>
-      <c r="F189" s="160">
+      <c r="F189" s="243">
         <f t="shared" si="31"/>
         <v>46.666618019999994</v>
       </c>
-      <c r="H189" s="32"/>
-    </row>
-    <row r="190" spans="2:8" outlineLevel="1">
+      <c r="H189" s="255">
+        <f>C189</f>
+        <v>40.808459999999997</v>
+      </c>
+      <c r="I189" s="260">
+        <f>D189-C189</f>
+        <v>1.7585700000000131</v>
+      </c>
+      <c r="J189" s="260">
+        <f t="shared" ref="J189:J192" si="32">E189-D189</f>
+        <v>1.8803208599999977</v>
+      </c>
+      <c r="K189" s="260">
+        <f t="shared" ref="K189:K192" si="33">F189-E189</f>
+        <v>2.2192671599999869</v>
+      </c>
+    </row>
+    <row r="190" spans="2:11" outlineLevel="1">
       <c r="B190" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="C190" s="158">
-        <f t="shared" ref="C190:F190" si="32">$C$153*MAX(0,C175)</f>
-        <v>0</v>
-      </c>
-      <c r="D190" s="161">
+      <c r="C190" s="243">
+        <f t="shared" ref="C190:F190" si="34">$C$153*MAX(0,C175)</f>
+        <v>0</v>
+      </c>
+      <c r="D190" s="244">
+        <f t="shared" si="34"/>
+        <v>42.56703000000001</v>
+      </c>
+      <c r="E190" s="243">
+        <f t="shared" si="34"/>
+        <v>44.385343200000001</v>
+      </c>
+      <c r="F190" s="243">
+        <f t="shared" si="34"/>
+        <v>45.100057364999998</v>
+      </c>
+      <c r="I190" s="260">
+        <f t="shared" ref="I190:I192" si="35">D190-C190</f>
+        <v>42.56703000000001</v>
+      </c>
+      <c r="J190" s="260">
         <f t="shared" si="32"/>
-        <v>42.56703000000001</v>
-      </c>
-      <c r="E190" s="160">
-        <f t="shared" si="32"/>
-        <v>44.385343200000001</v>
-      </c>
-      <c r="F190" s="160">
-        <f t="shared" si="32"/>
-        <v>45.100057364999998</v>
-      </c>
-    </row>
-    <row r="191" spans="2:8" outlineLevel="1">
+        <v>1.8183131999999915</v>
+      </c>
+      <c r="K190" s="260">
+        <f t="shared" si="33"/>
+        <v>0.71471416499999663</v>
+      </c>
+    </row>
+    <row r="191" spans="2:11" ht="14.4" outlineLevel="1">
       <c r="B191" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="C191" s="158">
-        <f t="shared" ref="C191:F191" si="33">$C$153*MAX(0,C176)</f>
-        <v>0</v>
-      </c>
-      <c r="D191" s="158">
+      <c r="C191" s="243">
+        <f t="shared" ref="C191:F191" si="36">$C$153*MAX(0,C176)</f>
+        <v>0</v>
+      </c>
+      <c r="D191" s="243">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="E191" s="244">
+        <f t="shared" si="36"/>
+        <v>31.475994</v>
+      </c>
+      <c r="F191" s="243">
+        <f t="shared" si="36"/>
+        <v>30.426392699999997</v>
+      </c>
+      <c r="I191" s="260">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="J191" s="260">
+        <f t="shared" si="32"/>
+        <v>31.475994</v>
+      </c>
+      <c r="K191" s="261">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="E191" s="161">
-        <f t="shared" si="33"/>
-        <v>31.475994</v>
-      </c>
-      <c r="F191" s="160">
-        <f t="shared" si="33"/>
-        <v>30.426392699999997</v>
-      </c>
-    </row>
-    <row r="192" spans="2:8" outlineLevel="1">
+        <v>-1.0496013000000026</v>
+      </c>
+    </row>
+    <row r="192" spans="2:11" outlineLevel="1">
       <c r="B192" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="C192" s="158">
-        <f t="shared" ref="C192:F192" si="34">$C$153*MAX(0,C177)</f>
-        <v>0</v>
-      </c>
-      <c r="D192" s="158">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="E192" s="158">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="F192" s="161">
-        <f t="shared" si="34"/>
+      <c r="C192" s="243">
+        <f t="shared" ref="C192:F192" si="37">$C$153*MAX(0,C177)</f>
+        <v>0</v>
+      </c>
+      <c r="D192" s="243">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="E192" s="243">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="F192" s="244">
+        <f t="shared" si="37"/>
+        <v>17.392979999999998</v>
+      </c>
+      <c r="I192" s="260">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="J192" s="260">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="K192" s="260">
+        <f t="shared" si="33"/>
         <v>17.392979999999998</v>
       </c>
     </row>
@@ -8954,20 +9030,20 @@
       <c r="B196" s="175" t="s">
         <v>112</v>
       </c>
-      <c r="C196" s="199">
+      <c r="C196" s="256">
         <f>C189+C181</f>
         <v>58.328459999999993</v>
       </c>
-      <c r="D196" s="200">
-        <f t="shared" ref="D196:F196" si="35">D189+D181</f>
+      <c r="D196" s="250">
+        <f t="shared" ref="D196:F196" si="38">D189+D181</f>
         <v>60.963030000000003</v>
       </c>
-      <c r="E196" s="200">
-        <f t="shared" si="35"/>
+      <c r="E196" s="250">
+        <f t="shared" si="38"/>
         <v>63.76315086000001</v>
       </c>
-      <c r="F196" s="200">
-        <f t="shared" si="35"/>
+      <c r="F196" s="250">
+        <f t="shared" si="38"/>
         <v>66.948208019999996</v>
       </c>
       <c r="H196" s="32"/>
@@ -8979,20 +9055,20 @@
       <c r="B197" s="175" t="s">
         <v>111</v>
       </c>
-      <c r="C197" s="201">
-        <f t="shared" ref="C197:F197" si="36">C190+C182</f>
-        <v>0</v>
-      </c>
-      <c r="D197" s="202">
-        <f t="shared" si="36"/>
+      <c r="C197" s="250">
+        <f t="shared" ref="C197:F197" si="39">C190+C182</f>
+        <v>0</v>
+      </c>
+      <c r="D197" s="252">
+        <f t="shared" si="39"/>
         <v>60.963030000000003</v>
       </c>
-      <c r="E197" s="200">
-        <f t="shared" si="36"/>
+      <c r="E197" s="250">
+        <f t="shared" si="39"/>
         <v>63.701143200000004</v>
       </c>
-      <c r="F197" s="200">
-        <f t="shared" si="36"/>
+      <c r="F197" s="250">
+        <f t="shared" si="39"/>
         <v>65.381647364999992</v>
       </c>
       <c r="H197" s="32"/>
@@ -9004,20 +9080,20 @@
       <c r="B198" s="175" t="s">
         <v>110</v>
       </c>
-      <c r="C198" s="201">
-        <f t="shared" ref="C198:F198" si="37">C191+C183</f>
-        <v>0</v>
-      </c>
-      <c r="D198" s="201">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="E198" s="202">
-        <f t="shared" si="37"/>
+      <c r="C198" s="250">
+        <f t="shared" ref="C198:F198" si="40">C191+C183</f>
+        <v>0</v>
+      </c>
+      <c r="D198" s="250">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="E198" s="252">
+        <f t="shared" si="40"/>
         <v>48.119993999999998</v>
       </c>
-      <c r="F198" s="200">
-        <f t="shared" si="37"/>
+      <c r="F198" s="250">
+        <f t="shared" si="40"/>
         <v>47.9025927</v>
       </c>
     </row>
@@ -9026,20 +9102,20 @@
       <c r="B199" s="175" t="s">
         <v>109</v>
       </c>
-      <c r="C199" s="201">
-        <f t="shared" ref="C199:F199" si="38">C192+C184</f>
-        <v>0</v>
-      </c>
-      <c r="D199" s="201">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="E199" s="201">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="F199" s="202">
-        <f t="shared" si="38"/>
+      <c r="C199" s="250">
+        <f t="shared" ref="C199:F199" si="41">C192+C184</f>
+        <v>0</v>
+      </c>
+      <c r="D199" s="250">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="E199" s="250">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="F199" s="252">
+        <f t="shared" si="41"/>
         <v>32.284979999999997</v>
       </c>
     </row>
@@ -9109,90 +9185,146 @@
         <v>113</v>
       </c>
     </row>
-    <row r="209" spans="2:7" ht="14.4" outlineLevel="1">
+    <row r="209" spans="2:12" ht="14.4" outlineLevel="1">
       <c r="B209" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="C209" s="253">
-        <v>59.348999999999997</v>
+      <c r="C209" s="259">
+        <v>58.33</v>
       </c>
       <c r="D209" s="243">
-        <f t="shared" ref="D209:F209" si="39">IF($C$203="profit",D196,IF($C$203="fix",D89,D144))</f>
+        <f t="shared" ref="C209:F209" si="42">IF($C$203="profit",D196,IF($C$203="fix",D89,D144))</f>
         <v>60.963030000000003</v>
       </c>
       <c r="E209" s="243">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>63.76315086000001</v>
       </c>
       <c r="F209" s="243">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>66.948208019999996</v>
       </c>
-    </row>
-    <row r="210" spans="2:7" outlineLevel="1">
+      <c r="H209" s="255">
+        <f>C209</f>
+        <v>58.33</v>
+      </c>
+      <c r="I209" s="260">
+        <f>D209-C209</f>
+        <v>2.6330300000000051</v>
+      </c>
+      <c r="J209" s="260">
+        <f t="shared" ref="J209:L212" si="43">E209-D209</f>
+        <v>2.8001208600000069</v>
+      </c>
+      <c r="K209" s="260">
+        <f t="shared" si="43"/>
+        <v>3.1850571599999853</v>
+      </c>
+      <c r="L209" s="260"/>
+    </row>
+    <row r="210" spans="2:12" outlineLevel="1">
       <c r="B210" s="122" t="s">
         <v>111</v>
       </c>
       <c r="C210" s="243">
-        <f t="shared" ref="C210:F210" si="40">IF($C$203="profit",C197,IF($C$203="fix",C90,C145))</f>
+        <f t="shared" ref="C210:F210" si="44">IF($C$203="profit",C197,IF($C$203="fix",C90,C145))</f>
         <v>0</v>
       </c>
       <c r="D210" s="244">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>60.963030000000003</v>
       </c>
       <c r="E210" s="243">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>63.701143200000004</v>
       </c>
       <c r="F210" s="243">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>65.381647364999992</v>
       </c>
-    </row>
-    <row r="211" spans="2:7" outlineLevel="1">
+      <c r="I210" s="260">
+        <f t="shared" ref="I210:I212" si="45">D210-C210</f>
+        <v>60.963030000000003</v>
+      </c>
+      <c r="J210" s="260">
+        <f t="shared" si="43"/>
+        <v>2.7381132000000008</v>
+      </c>
+      <c r="K210" s="260">
+        <f t="shared" si="43"/>
+        <v>1.6805041649999879</v>
+      </c>
+      <c r="L210" s="260"/>
+    </row>
+    <row r="211" spans="2:12" ht="14.4" outlineLevel="1">
       <c r="B211" s="122" t="s">
         <v>110</v>
       </c>
       <c r="C211" s="243">
-        <f t="shared" ref="C211:F211" si="41">IF($C$203="profit",C198,IF($C$203="fix",C91,C146))</f>
+        <f t="shared" ref="C211:F211" si="46">IF($C$203="profit",C198,IF($C$203="fix",C91,C146))</f>
         <v>0</v>
       </c>
       <c r="D211" s="243">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="E211" s="244">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>48.119993999999998</v>
       </c>
       <c r="F211" s="243">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>47.9025927</v>
       </c>
-    </row>
-    <row r="212" spans="2:7" outlineLevel="1">
+      <c r="I211" s="260">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="J211" s="260">
+        <f t="shared" si="43"/>
+        <v>48.119993999999998</v>
+      </c>
+      <c r="K211" s="261">
+        <f t="shared" si="43"/>
+        <v>-0.2174012999999988</v>
+      </c>
+      <c r="L211" s="260"/>
+    </row>
+    <row r="212" spans="2:12" outlineLevel="1">
       <c r="B212" s="122" t="s">
         <v>109</v>
       </c>
       <c r="C212" s="243">
-        <f t="shared" ref="C212:F212" si="42">IF($C$203="profit",C199,IF($C$203="fix",C92,C147))</f>
+        <f t="shared" ref="C212:F212" si="47">IF($C$203="profit",C199,IF($C$203="fix",C92,C147))</f>
         <v>0</v>
       </c>
       <c r="D212" s="243">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="E212" s="243">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F212" s="244">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>32.284979999999997</v>
       </c>
-    </row>
-    <row r="213" spans="2:7" outlineLevel="1">
+      <c r="I212" s="260">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="J212" s="260">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="K212" s="260">
+        <f t="shared" si="43"/>
+        <v>32.284979999999997</v>
+      </c>
+      <c r="L212" s="260"/>
+    </row>
+    <row r="213" spans="2:12" outlineLevel="1">
       <c r="B213" s="172"/>
       <c r="C213" s="250"/>
       <c r="D213" s="250"/>
@@ -9200,7 +9332,7 @@
       <c r="F213" s="250"/>
       <c r="G213" s="172"/>
     </row>
-    <row r="214" spans="2:7" ht="14.4" outlineLevel="1">
+    <row r="214" spans="2:12" ht="14.4" outlineLevel="1">
       <c r="B214" s="174" t="s">
         <v>236</v>
       </c>
@@ -9218,118 +9350,171 @@
       </c>
       <c r="G214" s="172"/>
     </row>
-    <row r="215" spans="2:7" ht="14.4" outlineLevel="1">
+    <row r="215" spans="2:12" outlineLevel="1">
       <c r="B215" s="175" t="s">
         <v>112</v>
       </c>
-      <c r="C215" s="245">
-        <v>40.81</v>
+      <c r="C215" s="250">
+        <f>IF($C$203="profit",C181,IF($C$203="fix",C89,C137))</f>
+        <v>17.52</v>
       </c>
       <c r="D215" s="250">
-        <f t="shared" ref="D215:F215" si="43">IF($C$203="profit",D189,IF($C$203="fix",D89,D137))</f>
-        <v>42.56703000000001</v>
+        <f>IF($C$203="profit",D181,IF($C$203="fix",D89,D137))</f>
+        <v>18.395999999999997</v>
       </c>
       <c r="E215" s="250">
-        <f t="shared" si="43"/>
-        <v>44.447350860000007</v>
+        <f>IF($C$203="profit",E181,IF($C$203="fix",E89,E137))</f>
+        <v>19.315799999999999</v>
       </c>
       <c r="F215" s="250">
-        <f t="shared" si="43"/>
-        <v>46.666618019999994</v>
+        <f>IF($C$203="profit",F181,IF($C$203="fix",F89,F137))</f>
+        <v>20.281589999999998</v>
       </c>
       <c r="G215" s="172"/>
-    </row>
-    <row r="216" spans="2:7" outlineLevel="1">
+      <c r="H215" s="255">
+        <f>C215</f>
+        <v>17.52</v>
+      </c>
+      <c r="I215" s="260">
+        <f>D215-C215</f>
+        <v>0.87599999999999767</v>
+      </c>
+      <c r="J215" s="260">
+        <f t="shared" ref="J215:J218" si="48">E215-D215</f>
+        <v>0.91980000000000217</v>
+      </c>
+      <c r="K215" s="260">
+        <f t="shared" ref="K215:K218" si="49">F215-E215</f>
+        <v>0.96578999999999837</v>
+      </c>
+    </row>
+    <row r="216" spans="2:12" outlineLevel="1">
       <c r="B216" s="175" t="s">
         <v>111</v>
       </c>
       <c r="C216" s="250">
-        <f t="shared" ref="C216:F216" si="44">IF($C$203="profit",C190,IF($C$203="fix",C90,C138))</f>
-        <v>0</v>
-      </c>
-      <c r="D216" s="252">
-        <f t="shared" si="44"/>
-        <v>42.56703000000001</v>
+        <f t="shared" ref="C216:F216" si="50">IF($C$203="profit",C190,IF($C$203="fix",C90,C138))</f>
+        <v>0</v>
+      </c>
+      <c r="D216" s="250">
+        <f>IF($C$203="profit",D182,IF($C$203="fix",D90,D138))</f>
+        <v>18.395999999999997</v>
       </c>
       <c r="E216" s="250">
-        <f t="shared" si="44"/>
-        <v>44.385343200000001</v>
+        <f>IF($C$203="profit",E182,IF($C$203="fix",E90,E138))</f>
+        <v>19.315799999999999</v>
       </c>
       <c r="F216" s="250">
-        <f t="shared" si="44"/>
-        <v>45.100057364999998</v>
+        <f>IF($C$203="profit",F182,IF($C$203="fix",F90,F138))</f>
+        <v>20.281589999999998</v>
       </c>
       <c r="G216" s="172"/>
-    </row>
-    <row r="217" spans="2:7" outlineLevel="1">
+      <c r="I216" s="260">
+        <f t="shared" ref="I216:I218" si="51">D216-C216</f>
+        <v>18.395999999999997</v>
+      </c>
+      <c r="J216" s="260">
+        <f t="shared" si="48"/>
+        <v>0.91980000000000217</v>
+      </c>
+      <c r="K216" s="260">
+        <f t="shared" si="49"/>
+        <v>0.96578999999999837</v>
+      </c>
+    </row>
+    <row r="217" spans="2:12" ht="14.4" outlineLevel="1">
       <c r="B217" s="175" t="s">
         <v>110</v>
       </c>
       <c r="C217" s="250">
-        <f t="shared" ref="C217:F217" si="45">IF($C$203="profit",C191,IF($C$203="fix",C91,C139))</f>
+        <f t="shared" ref="C217:F217" si="52">IF($C$203="profit",C191,IF($C$203="fix",C91,C139))</f>
         <v>0</v>
       </c>
       <c r="D217" s="250">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="E217" s="252">
-        <f t="shared" si="45"/>
-        <v>31.475994</v>
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="E217" s="250">
+        <f>IF($C$203="profit",E183,IF($C$203="fix",E91,E139))</f>
+        <v>16.643999999999998</v>
       </c>
       <c r="F217" s="250">
-        <f t="shared" si="45"/>
-        <v>30.426392699999997</v>
+        <f>IF($C$203="profit",F183,IF($C$203="fix",F91,F139))</f>
+        <v>17.476199999999999</v>
       </c>
       <c r="G217" s="172"/>
-    </row>
-    <row r="218" spans="2:7" outlineLevel="1">
+      <c r="I217" s="260">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="J217" s="260">
+        <f t="shared" si="48"/>
+        <v>16.643999999999998</v>
+      </c>
+      <c r="K217" s="261">
+        <f t="shared" si="49"/>
+        <v>0.83220000000000027</v>
+      </c>
+    </row>
+    <row r="218" spans="2:12" outlineLevel="1">
       <c r="B218" s="175" t="s">
         <v>109</v>
       </c>
       <c r="C218" s="250">
-        <f t="shared" ref="C218:F218" si="46">IF($C$203="profit",C192,IF($C$203="fix",C92,C140))</f>
+        <f t="shared" ref="C218:F218" si="53">IF($C$203="profit",C192,IF($C$203="fix",C92,C140))</f>
         <v>0</v>
       </c>
       <c r="D218" s="250">
-        <f t="shared" si="46"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="E218" s="250">
-        <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="F218" s="252">
-        <f t="shared" si="46"/>
-        <v>17.392979999999998</v>
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="F218" s="250">
+        <f>IF($C$203="profit",F184,IF($C$203="fix",F92,F140))</f>
+        <v>14.891999999999999</v>
       </c>
       <c r="G218" s="172"/>
-    </row>
-    <row r="219" spans="2:7" outlineLevel="1">
+      <c r="I218" s="260">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="J218" s="260">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="K218" s="260">
+        <f t="shared" si="49"/>
+        <v>14.891999999999999</v>
+      </c>
+    </row>
+    <row r="219" spans="2:12" outlineLevel="1">
       <c r="C219" s="158"/>
       <c r="D219" s="158"/>
       <c r="E219" s="158"/>
       <c r="F219" s="162"/>
     </row>
-    <row r="220" spans="2:7" outlineLevel="1">
+    <row r="220" spans="2:12" outlineLevel="1">
       <c r="B220" s="22"/>
       <c r="F220" s="130"/>
     </row>
-    <row r="221" spans="2:7" outlineLevel="1">
+    <row r="221" spans="2:12" outlineLevel="1">
       <c r="C221" s="158"/>
       <c r="D221" s="158"/>
       <c r="E221" s="158"/>
       <c r="F221" s="162"/>
     </row>
-    <row r="222" spans="2:7" s="149" customFormat="1" ht="15.6" outlineLevel="1">
+    <row r="222" spans="2:12" s="149" customFormat="1" ht="15.6" outlineLevel="1">
       <c r="B222" s="150" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="223" spans="2:7" outlineLevel="1">
+    <row r="223" spans="2:12" outlineLevel="1">
       <c r="B223"/>
     </row>
-    <row r="224" spans="2:7" ht="14.4" outlineLevel="1">
+    <row r="224" spans="2:12" ht="14.4" outlineLevel="1">
       <c r="B224" s="123" t="s">
         <v>230</v>
       </c>
@@ -9355,15 +9540,15 @@
         <v>-146</v>
       </c>
       <c r="D225" s="160">
-        <f t="shared" ref="D225:F225" si="47">-$C$22*D16</f>
+        <f t="shared" ref="D225:F225" si="54">-$C$22*D16</f>
         <v>-153.29999999999998</v>
       </c>
       <c r="E225" s="160">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v>-160.965</v>
       </c>
       <c r="F225" s="160">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v>-169.01325</v>
       </c>
       <c r="H225" t="s">
@@ -9375,19 +9560,19 @@
         <v>111</v>
       </c>
       <c r="C226" s="158">
-        <f t="shared" ref="C226:F226" si="48">-$C$22*C17</f>
+        <f t="shared" ref="C226:F226" si="55">-$C$22*C17</f>
         <v>0</v>
       </c>
       <c r="D226" s="161">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>-153.29999999999998</v>
       </c>
       <c r="E226" s="160">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>-160.965</v>
       </c>
       <c r="F226" s="160">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>-169.01325</v>
       </c>
     </row>
@@ -9396,19 +9581,19 @@
         <v>110</v>
       </c>
       <c r="C227" s="158">
-        <f t="shared" ref="C227:F227" si="49">-$C$22*C18</f>
+        <f t="shared" ref="C227:F227" si="56">-$C$22*C18</f>
         <v>0</v>
       </c>
       <c r="D227" s="158">
-        <f t="shared" si="49"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="E227" s="161">
-        <f t="shared" si="49"/>
+        <f t="shared" si="56"/>
         <v>-138.69999999999999</v>
       </c>
       <c r="F227" s="160">
-        <f t="shared" si="49"/>
+        <f t="shared" si="56"/>
         <v>-145.63499999999999</v>
       </c>
     </row>
@@ -9417,19 +9602,19 @@
         <v>109</v>
       </c>
       <c r="C228" s="158">
-        <f t="shared" ref="C228:F228" si="50">-$C$22*C19</f>
+        <f t="shared" ref="C228:F228" si="57">-$C$22*C19</f>
         <v>0</v>
       </c>
       <c r="D228" s="158">
-        <f t="shared" si="50"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="E228" s="158">
-        <f t="shared" si="50"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="F228" s="161">
-        <f t="shared" si="50"/>
+        <f t="shared" si="57"/>
         <v>-124.1</v>
       </c>
     </row>
@@ -9465,15 +9650,15 @@
         <v>54</v>
       </c>
       <c r="D232" s="160">
-        <f t="shared" ref="D232:F232" si="51">D16+D225</f>
+        <f t="shared" ref="D232:F232" si="58">D16+D225</f>
         <v>56.700000000000017</v>
       </c>
       <c r="E232" s="160">
-        <f t="shared" si="51"/>
+        <f t="shared" si="58"/>
         <v>59.534999999999997</v>
       </c>
       <c r="F232" s="160">
-        <f t="shared" si="51"/>
+        <f t="shared" si="58"/>
         <v>62.511750000000006</v>
       </c>
     </row>
@@ -9482,19 +9667,19 @@
         <v>111</v>
       </c>
       <c r="C233" s="158">
-        <f t="shared" ref="C233:F233" si="52">C17+C226</f>
+        <f t="shared" ref="C233:F233" si="59">C17+C226</f>
         <v>0</v>
       </c>
       <c r="D233" s="161">
-        <f t="shared" si="52"/>
+        <f t="shared" si="59"/>
         <v>56.700000000000017</v>
       </c>
       <c r="E233" s="160">
-        <f t="shared" si="52"/>
+        <f t="shared" si="59"/>
         <v>59.534999999999997</v>
       </c>
       <c r="F233" s="160">
-        <f t="shared" si="52"/>
+        <f t="shared" si="59"/>
         <v>62.511750000000006</v>
       </c>
     </row>
@@ -9503,19 +9688,19 @@
         <v>110</v>
       </c>
       <c r="C234" s="158">
-        <f t="shared" ref="C234:F234" si="53">C18+C227</f>
+        <f t="shared" ref="C234:F234" si="60">C18+C227</f>
         <v>0</v>
       </c>
       <c r="D234" s="158">
-        <f t="shared" si="53"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="E234" s="161">
-        <f t="shared" si="53"/>
+        <f t="shared" si="60"/>
         <v>51.300000000000011</v>
       </c>
       <c r="F234" s="160">
-        <f t="shared" si="53"/>
+        <f t="shared" si="60"/>
         <v>53.865000000000009</v>
       </c>
     </row>
@@ -9524,19 +9709,19 @@
         <v>109</v>
       </c>
       <c r="C235" s="158">
-        <f t="shared" ref="C235:F235" si="54">C19+C228</f>
+        <f t="shared" ref="C235:F235" si="61">C19+C228</f>
         <v>0</v>
       </c>
       <c r="D235" s="158">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="E235" s="158">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="F235" s="161">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>45.900000000000006</v>
       </c>
     </row>
@@ -9583,15 +9768,15 @@
         <v>-90</v>
       </c>
       <c r="D241" s="220">
-        <f t="shared" ref="D241:F241" si="55">D10</f>
+        <f t="shared" ref="D241:F241" si="62">D10</f>
         <v>-99</v>
       </c>
       <c r="E241" s="220">
-        <f t="shared" si="55"/>
+        <f t="shared" si="62"/>
         <v>-107.91</v>
       </c>
       <c r="F241" s="220">
-        <f t="shared" si="55"/>
+        <f t="shared" si="62"/>
         <v>-113.35499999999999</v>
       </c>
       <c r="H241" s="167"/>
@@ -9601,19 +9786,19 @@
         <v>111</v>
       </c>
       <c r="C242" s="220">
-        <f t="shared" ref="C242:F242" si="56">C11</f>
+        <f t="shared" ref="C242:F242" si="63">C11</f>
         <v>0</v>
       </c>
       <c r="D242" s="221">
-        <f t="shared" si="56"/>
+        <f t="shared" si="63"/>
         <v>-99</v>
       </c>
       <c r="E242" s="220">
-        <f t="shared" si="56"/>
+        <f t="shared" si="63"/>
         <v>-108.9</v>
       </c>
       <c r="F242" s="220">
-        <f t="shared" si="56"/>
+        <f t="shared" si="63"/>
         <v>-118.70100000000001</v>
       </c>
       <c r="H242" s="167"/>
@@ -9623,19 +9808,19 @@
         <v>110</v>
       </c>
       <c r="C243" s="220">
-        <f t="shared" ref="C243:F243" si="57">C12</f>
+        <f t="shared" ref="C243:F243" si="64">C12</f>
         <v>0</v>
       </c>
       <c r="D243" s="220">
-        <f t="shared" si="57"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="E243" s="221">
-        <f t="shared" si="57"/>
+        <f t="shared" si="64"/>
         <v>-108.9</v>
       </c>
       <c r="F243" s="220">
-        <f t="shared" si="57"/>
+        <f t="shared" si="64"/>
         <v>-119.79</v>
       </c>
       <c r="H243" s="167"/>
@@ -9645,19 +9830,19 @@
         <v>109</v>
       </c>
       <c r="C244" s="220">
-        <f t="shared" ref="C244:F244" si="58">C13</f>
+        <f t="shared" ref="C244:F244" si="65">C13</f>
         <v>0</v>
       </c>
       <c r="D244" s="220">
-        <f t="shared" si="58"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="E244" s="220">
-        <f t="shared" si="58"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="F244" s="221">
-        <f t="shared" si="58"/>
+        <f t="shared" si="65"/>
         <v>-119.79</v>
       </c>
       <c r="H244" s="167"/>
@@ -9697,15 +9882,15 @@
         <v>59.348999999999997</v>
       </c>
       <c r="D247" s="249">
-        <f t="shared" ref="D247:F247" si="59">D78*D16*$C$22</f>
+        <f t="shared" ref="D247:F247" si="66">D78*D16*$C$22</f>
         <v>62.743499999999997</v>
       </c>
       <c r="E247" s="249">
-        <f t="shared" si="59"/>
+        <f t="shared" si="66"/>
         <v>66.256479000000013</v>
       </c>
       <c r="F247" s="249">
-        <f t="shared" si="59"/>
+        <f t="shared" si="66"/>
         <v>69.574000500000011</v>
       </c>
     </row>
@@ -9714,11 +9899,11 @@
         <v>111</v>
       </c>
       <c r="C248" s="243">
-        <f t="shared" ref="C248:F248" si="60">C79*C17*$C$22</f>
+        <f t="shared" ref="C248:F248" si="67">C79*C17*$C$22</f>
         <v>0</v>
       </c>
       <c r="D248" s="244">
-        <f t="shared" si="60"/>
+        <f t="shared" si="67"/>
         <v>62.743499999999997</v>
       </c>
       <c r="E248" s="249">
@@ -9726,7 +9911,7 @@
         <v>66.350430000000003</v>
       </c>
       <c r="F248" s="249">
-        <f t="shared" si="60"/>
+        <f t="shared" si="67"/>
         <v>71.947577250000023</v>
       </c>
       <c r="H248" s="167"/>
@@ -9736,19 +9921,19 @@
         <v>110</v>
       </c>
       <c r="C249" s="243">
-        <f t="shared" ref="C249:F249" si="61">C80*C18*$C$22</f>
+        <f t="shared" ref="C249:F249" si="68">C80*C18*$C$22</f>
         <v>0</v>
       </c>
       <c r="D249" s="243">
-        <f t="shared" si="61"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="E249" s="244">
-        <f t="shared" si="61"/>
+        <f t="shared" si="68"/>
         <v>67.430099999999996</v>
       </c>
       <c r="F249" s="249">
-        <f t="shared" si="61"/>
+        <f t="shared" si="68"/>
         <v>74.776454999999999</v>
       </c>
       <c r="H249" s="167"/>
@@ -9758,19 +9943,19 @@
         <v>109</v>
       </c>
       <c r="C250" s="243">
-        <f t="shared" ref="C250:F250" si="62">C81*C19*$C$22</f>
+        <f t="shared" ref="C250:F250" si="69">C81*C19*$C$22</f>
         <v>0</v>
       </c>
       <c r="D250" s="243">
-        <f t="shared" si="62"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="E250" s="243">
-        <f t="shared" si="62"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="F250" s="244">
-        <f t="shared" si="62"/>
+        <f t="shared" si="69"/>
         <v>76.649999999999991</v>
       </c>
       <c r="H250" s="167"/>
@@ -9812,15 +9997,15 @@
         <v>-30.651000000000003</v>
       </c>
       <c r="D253" s="220">
-        <f t="shared" ref="D253:F253" si="63">D241+D247</f>
+        <f t="shared" ref="D253:F253" si="70">D241+D247</f>
         <v>-36.256500000000003</v>
       </c>
       <c r="E253" s="220">
-        <f t="shared" si="63"/>
+        <f t="shared" si="70"/>
         <v>-41.653520999999984</v>
       </c>
       <c r="F253" s="220">
-        <f t="shared" si="63"/>
+        <f t="shared" si="70"/>
         <v>-43.780999499999979</v>
       </c>
     </row>
@@ -9829,19 +10014,19 @@
         <v>111</v>
       </c>
       <c r="C254" s="220">
-        <f t="shared" ref="C254:F254" si="64">C242+C248</f>
+        <f t="shared" ref="C254:F254" si="71">C242+C248</f>
         <v>0</v>
       </c>
       <c r="D254" s="221">
-        <f t="shared" si="64"/>
+        <f t="shared" si="71"/>
         <v>-36.256500000000003</v>
       </c>
       <c r="E254" s="220">
-        <f t="shared" si="64"/>
+        <f t="shared" si="71"/>
         <v>-42.549570000000003</v>
       </c>
       <c r="F254" s="220">
-        <f t="shared" si="64"/>
+        <f t="shared" si="71"/>
         <v>-46.753422749999984</v>
       </c>
     </row>
@@ -9850,19 +10035,19 @@
         <v>110</v>
       </c>
       <c r="C255" s="220">
-        <f t="shared" ref="C255:F255" si="65">C243+C249</f>
+        <f t="shared" ref="C255:F255" si="72">C243+C249</f>
         <v>0</v>
       </c>
       <c r="D255" s="220">
-        <f t="shared" si="65"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="E255" s="221">
-        <f t="shared" si="65"/>
+        <f t="shared" si="72"/>
         <v>-41.46990000000001</v>
       </c>
       <c r="F255" s="220">
-        <f t="shared" si="65"/>
+        <f t="shared" si="72"/>
         <v>-45.013545000000008</v>
       </c>
     </row>
@@ -9871,19 +10056,19 @@
         <v>109</v>
       </c>
       <c r="C256" s="220">
-        <f t="shared" ref="C256:F256" si="66">C244+C250</f>
+        <f t="shared" ref="C256:F256" si="73">C244+C250</f>
         <v>0</v>
       </c>
       <c r="D256" s="220">
-        <f t="shared" si="66"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="E256" s="220">
-        <f t="shared" si="66"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="F256" s="221">
-        <f t="shared" si="66"/>
+        <f t="shared" si="73"/>
         <v>-43.140000000000015</v>
       </c>
     </row>
@@ -9919,18 +10104,18 @@
       </c>
       <c r="C259" s="159">
         <f>C253+C209+C232</f>
-        <v>82.697999999999993</v>
+        <v>81.679000000000002</v>
       </c>
       <c r="D259" s="160">
-        <f t="shared" ref="D259:F259" si="67">D253+D209+D232</f>
+        <f t="shared" ref="D259:F259" si="74">D253+D209+D232</f>
         <v>81.406530000000018</v>
       </c>
       <c r="E259" s="160">
-        <f t="shared" si="67"/>
+        <f t="shared" si="74"/>
         <v>81.644629860000023</v>
       </c>
       <c r="F259" s="160">
-        <f t="shared" si="67"/>
+        <f t="shared" si="74"/>
         <v>85.678958520000023</v>
       </c>
     </row>
@@ -9939,19 +10124,19 @@
         <v>111</v>
       </c>
       <c r="C260" s="158">
-        <f t="shared" ref="C260:F260" si="68">C254+C210+C233</f>
+        <f t="shared" ref="C260:F260" si="75">C254+C210+C233</f>
         <v>0</v>
       </c>
       <c r="D260" s="161">
-        <f t="shared" si="68"/>
+        <f t="shared" si="75"/>
         <v>81.406530000000018</v>
       </c>
       <c r="E260" s="160">
-        <f t="shared" si="68"/>
+        <f t="shared" si="75"/>
         <v>80.686573199999998</v>
       </c>
       <c r="F260" s="160">
-        <f t="shared" si="68"/>
+        <f t="shared" si="75"/>
         <v>81.139974615000014</v>
       </c>
     </row>
@@ -9960,19 +10145,19 @@
         <v>110</v>
       </c>
       <c r="C261" s="158">
-        <f t="shared" ref="C261:F261" si="69">C255+C211+C234</f>
+        <f t="shared" ref="C261:F261" si="76">C255+C211+C234</f>
         <v>0</v>
       </c>
       <c r="D261" s="158">
-        <f t="shared" si="69"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E261" s="161">
-        <f t="shared" si="69"/>
+        <f t="shared" si="76"/>
         <v>57.950094</v>
       </c>
       <c r="F261" s="160">
-        <f t="shared" si="69"/>
+        <f t="shared" si="76"/>
         <v>56.754047700000001</v>
       </c>
     </row>
@@ -9981,19 +10166,19 @@
         <v>109</v>
       </c>
       <c r="C262" s="158">
-        <f t="shared" ref="C262:F262" si="70">C256+C212+C235</f>
+        <f t="shared" ref="C262:F262" si="77">C256+C212+C235</f>
         <v>0</v>
       </c>
       <c r="D262" s="158">
-        <f t="shared" si="70"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="E262" s="158">
-        <f t="shared" si="70"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F262" s="161">
-        <f t="shared" si="70"/>
+        <f t="shared" si="77"/>
         <v>35.044979999999988</v>
       </c>
     </row>
@@ -10023,18 +10208,18 @@
       </c>
       <c r="C265" s="159">
         <f>C259</f>
-        <v>82.697999999999993</v>
+        <v>81.679000000000002</v>
       </c>
       <c r="D265" s="160">
         <f>D259-C259</f>
-        <v>-1.2914699999999755</v>
+        <v>-0.27246999999998422</v>
       </c>
       <c r="E265" s="160">
-        <f t="shared" ref="E265:F266" si="71">E259-D259</f>
+        <f t="shared" ref="E265:F266" si="78">E259-D259</f>
         <v>0.23809986000000549</v>
       </c>
       <c r="F265" s="160">
-        <f t="shared" si="71"/>
+        <f t="shared" si="78"/>
         <v>4.0343286599999999</v>
       </c>
     </row>
@@ -10048,11 +10233,11 @@
         <v>81.406530000000018</v>
       </c>
       <c r="E266" s="160">
-        <f t="shared" si="71"/>
+        <f t="shared" si="78"/>
         <v>-0.71995680000001983</v>
       </c>
       <c r="F266" s="160">
-        <f t="shared" si="71"/>
+        <f t="shared" si="78"/>
         <v>0.45340141500001607</v>
       </c>
     </row>
@@ -10067,7 +10252,7 @@
         <v>57.950094</v>
       </c>
       <c r="F267" s="160">
-        <f t="shared" ref="F267" si="72">F261-E261</f>
+        <f t="shared" ref="F267" si="79">F261-E261</f>
         <v>-1.196046299999999</v>
       </c>
     </row>
@@ -10111,7 +10296,7 @@
       </c>
       <c r="C273" s="179">
         <f>C265</f>
-        <v>82.697999999999993</v>
+        <v>81.679000000000002</v>
       </c>
       <c r="D273" s="179">
         <f>D266</f>
@@ -10136,14 +10321,14 @@
       </c>
       <c r="D274" s="188">
         <f>SUM(D275:D278)</f>
-        <v>-1.2914699999999755</v>
+        <v>-0.27246999999998422</v>
       </c>
       <c r="E274" s="188">
-        <f t="shared" ref="E274:F274" si="73">SUM(E275:E278)</f>
+        <f t="shared" ref="E274:F274" si="80">SUM(E275:E278)</f>
         <v>-0.48185694000001433</v>
       </c>
       <c r="F274" s="188">
-        <f t="shared" si="73"/>
+        <f t="shared" si="80"/>
         <v>3.291683775000017</v>
       </c>
     </row>
@@ -10154,14 +10339,14 @@
       <c r="C275" s="181"/>
       <c r="D275" s="186">
         <f>D265</f>
-        <v>-1.2914699999999755</v>
+        <v>-0.27246999999998422</v>
       </c>
       <c r="E275" s="186">
-        <f t="shared" ref="E275:F275" si="74">E265</f>
+        <f t="shared" ref="E275:F275" si="81">E265</f>
         <v>0.23809986000000549</v>
       </c>
       <c r="F275" s="186">
-        <f t="shared" si="74"/>
+        <f t="shared" si="81"/>
         <v>4.0343286599999999</v>
       </c>
     </row>
@@ -10207,11 +10392,11 @@
       </c>
       <c r="C279" s="182">
         <f>C273+C274</f>
-        <v>82.697999999999993</v>
+        <v>81.679000000000002</v>
       </c>
       <c r="D279" s="182">
         <f>D273+D274</f>
-        <v>80.115060000000042</v>
+        <v>81.134060000000034</v>
       </c>
       <c r="E279" s="182">
         <f>E273+E274</f>

</xml_diff>

<commit_message>
PMO-2298: fixed loss carry forward with correct resetting and ordered application of period contract instances, further fixes in sliding commission calculation
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/PMO-2198_a___SSC_usual.xlsx
+++ b/test/data/spreadsheets/PMO-2198_a___SSC_usual.xlsx
@@ -985,7 +985,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -995,7 +995,8 @@
     <numFmt numFmtId="170" formatCode="#,##0.0;\-#,##0.00;"/>
     <numFmt numFmtId="171" formatCode="#,##0.00;\-#,##0.00;0.00"/>
     <numFmt numFmtId="172" formatCode="#,##0.000;\-#,##0.000;0.000"/>
-    <numFmt numFmtId="187" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
+    <numFmt numFmtId="173" formatCode="#,##0.000_ ;\-#,##0.000\ "/>
+    <numFmt numFmtId="174" formatCode="#,##0.0000000000;\-#,##0.0000000000;0.0000000000"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -1822,9 +1823,9 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="16" fillId="12" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="14" fillId="10" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="14" fillId="10" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="14" fillId="10" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="14" fillId="10" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2496,25 +2497,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="52091520"/>
-        <c:axId val="53612928"/>
+        <c:axId val="48882432"/>
+        <c:axId val="48883968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52091520"/>
+        <c:axId val="48882432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53612928"/>
+        <c:crossAx val="48883968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53612928"/>
+        <c:axId val="48883968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2522,7 +2523,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52091520"/>
+        <c:crossAx val="48882432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2534,7 +2535,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2816,11 +2817,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="54863360"/>
-        <c:axId val="54870016"/>
+        <c:axId val="48704896"/>
+        <c:axId val="48961024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54863360"/>
+        <c:axId val="48704896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2841,17 +2842,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54870016"/>
+        <c:crossAx val="48961024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54870016"/>
+        <c:axId val="48961024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2873,11 +2873,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54863360"/>
+        <c:crossAx val="48704896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5501,7 +5500,7 @@
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2784" topLeftCell="A185" activePane="bottomLeft"/>
       <selection activeCell="C215" sqref="C215"/>
-      <selection pane="bottomLeft" activeCell="K191" sqref="K191"/>
+      <selection pane="bottomLeft" activeCell="H189" sqref="H189:K192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -8874,15 +8873,15 @@
         <f>C189</f>
         <v>40.808459999999997</v>
       </c>
-      <c r="I189" s="260">
+      <c r="I189" s="259">
         <f>D189-C189</f>
         <v>1.7585700000000131</v>
       </c>
-      <c r="J189" s="260">
+      <c r="J189" s="259">
         <f t="shared" ref="J189:J192" si="32">E189-D189</f>
         <v>1.8803208599999977</v>
       </c>
-      <c r="K189" s="260">
+      <c r="K189" s="259">
         <f t="shared" ref="K189:K192" si="33">F189-E189</f>
         <v>2.2192671599999869</v>
       </c>
@@ -8907,15 +8906,15 @@
         <f t="shared" si="34"/>
         <v>45.100057364999998</v>
       </c>
-      <c r="I190" s="260">
+      <c r="I190" s="259">
         <f t="shared" ref="I190:I192" si="35">D190-C190</f>
         <v>42.56703000000001</v>
       </c>
-      <c r="J190" s="260">
+      <c r="J190" s="259">
         <f t="shared" si="32"/>
         <v>1.8183131999999915</v>
       </c>
-      <c r="K190" s="260">
+      <c r="K190" s="259">
         <f t="shared" si="33"/>
         <v>0.71471416499999663</v>
       </c>
@@ -8940,15 +8939,15 @@
         <f t="shared" si="36"/>
         <v>30.426392699999997</v>
       </c>
-      <c r="I191" s="260">
+      <c r="I191" s="259">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="J191" s="260">
+      <c r="J191" s="259">
         <f t="shared" si="32"/>
         <v>31.475994</v>
       </c>
-      <c r="K191" s="261">
+      <c r="K191" s="260">
         <f t="shared" si="33"/>
         <v>-1.0496013000000026</v>
       </c>
@@ -8973,15 +8972,15 @@
         <f t="shared" si="37"/>
         <v>17.392979999999998</v>
       </c>
-      <c r="I192" s="260">
+      <c r="I192" s="259">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="J192" s="260">
+      <c r="J192" s="259">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="K192" s="260">
+      <c r="K192" s="259">
         <f t="shared" si="33"/>
         <v>17.392979999999998</v>
       </c>
@@ -9189,11 +9188,11 @@
       <c r="B209" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="C209" s="259">
-        <v>58.33</v>
+      <c r="C209" s="261">
+        <v>58.32846</v>
       </c>
       <c r="D209" s="243">
-        <f t="shared" ref="C209:F209" si="42">IF($C$203="profit",D196,IF($C$203="fix",D89,D144))</f>
+        <f t="shared" ref="D209:F209" si="42">IF($C$203="profit",D196,IF($C$203="fix",D89,D144))</f>
         <v>60.963030000000003</v>
       </c>
       <c r="E209" s="243">
@@ -9206,21 +9205,21 @@
       </c>
       <c r="H209" s="255">
         <f>C209</f>
-        <v>58.33</v>
-      </c>
-      <c r="I209" s="260">
+        <v>58.32846</v>
+      </c>
+      <c r="I209" s="259">
         <f>D209-C209</f>
-        <v>2.6330300000000051</v>
-      </c>
-      <c r="J209" s="260">
-        <f t="shared" ref="J209:L212" si="43">E209-D209</f>
+        <v>2.6345700000000036</v>
+      </c>
+      <c r="J209" s="259">
+        <f t="shared" ref="J209:K212" si="43">E209-D209</f>
         <v>2.8001208600000069</v>
       </c>
-      <c r="K209" s="260">
+      <c r="K209" s="259">
         <f t="shared" si="43"/>
         <v>3.1850571599999853</v>
       </c>
-      <c r="L209" s="260"/>
+      <c r="L209" s="259"/>
     </row>
     <row r="210" spans="2:12" outlineLevel="1">
       <c r="B210" s="122" t="s">
@@ -9242,19 +9241,19 @@
         <f t="shared" si="44"/>
         <v>65.381647364999992</v>
       </c>
-      <c r="I210" s="260">
+      <c r="I210" s="259">
         <f t="shared" ref="I210:I212" si="45">D210-C210</f>
         <v>60.963030000000003</v>
       </c>
-      <c r="J210" s="260">
+      <c r="J210" s="259">
         <f t="shared" si="43"/>
         <v>2.7381132000000008</v>
       </c>
-      <c r="K210" s="260">
+      <c r="K210" s="259">
         <f t="shared" si="43"/>
         <v>1.6805041649999879</v>
       </c>
-      <c r="L210" s="260"/>
+      <c r="L210" s="259"/>
     </row>
     <row r="211" spans="2:12" ht="14.4" outlineLevel="1">
       <c r="B211" s="122" t="s">
@@ -9276,19 +9275,19 @@
         <f t="shared" si="46"/>
         <v>47.9025927</v>
       </c>
-      <c r="I211" s="260">
+      <c r="I211" s="259">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="J211" s="260">
+      <c r="J211" s="259">
         <f t="shared" si="43"/>
         <v>48.119993999999998</v>
       </c>
-      <c r="K211" s="261">
+      <c r="K211" s="260">
         <f t="shared" si="43"/>
         <v>-0.2174012999999988</v>
       </c>
-      <c r="L211" s="260"/>
+      <c r="L211" s="259"/>
     </row>
     <row r="212" spans="2:12" outlineLevel="1">
       <c r="B212" s="122" t="s">
@@ -9310,19 +9309,19 @@
         <f t="shared" si="47"/>
         <v>32.284979999999997</v>
       </c>
-      <c r="I212" s="260">
+      <c r="I212" s="259">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="J212" s="260">
+      <c r="J212" s="259">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="K212" s="260">
+      <c r="K212" s="259">
         <f t="shared" si="43"/>
         <v>32.284979999999997</v>
       </c>
-      <c r="L212" s="260"/>
+      <c r="L212" s="259"/>
     </row>
     <row r="213" spans="2:12" outlineLevel="1">
       <c r="B213" s="172"/>
@@ -9375,15 +9374,15 @@
         <f>C215</f>
         <v>17.52</v>
       </c>
-      <c r="I215" s="260">
+      <c r="I215" s="259">
         <f>D215-C215</f>
         <v>0.87599999999999767</v>
       </c>
-      <c r="J215" s="260">
+      <c r="J215" s="259">
         <f t="shared" ref="J215:J218" si="48">E215-D215</f>
         <v>0.91980000000000217</v>
       </c>
-      <c r="K215" s="260">
+      <c r="K215" s="259">
         <f t="shared" ref="K215:K218" si="49">F215-E215</f>
         <v>0.96578999999999837</v>
       </c>
@@ -9393,7 +9392,7 @@
         <v>111</v>
       </c>
       <c r="C216" s="250">
-        <f t="shared" ref="C216:F216" si="50">IF($C$203="profit",C190,IF($C$203="fix",C90,C138))</f>
+        <f t="shared" ref="C216" si="50">IF($C$203="profit",C190,IF($C$203="fix",C90,C138))</f>
         <v>0</v>
       </c>
       <c r="D216" s="250">
@@ -9409,15 +9408,15 @@
         <v>20.281589999999998</v>
       </c>
       <c r="G216" s="172"/>
-      <c r="I216" s="260">
+      <c r="I216" s="259">
         <f t="shared" ref="I216:I218" si="51">D216-C216</f>
         <v>18.395999999999997</v>
       </c>
-      <c r="J216" s="260">
+      <c r="J216" s="259">
         <f t="shared" si="48"/>
         <v>0.91980000000000217</v>
       </c>
-      <c r="K216" s="260">
+      <c r="K216" s="259">
         <f t="shared" si="49"/>
         <v>0.96578999999999837</v>
       </c>
@@ -9427,7 +9426,7 @@
         <v>110</v>
       </c>
       <c r="C217" s="250">
-        <f t="shared" ref="C217:F217" si="52">IF($C$203="profit",C191,IF($C$203="fix",C91,C139))</f>
+        <f t="shared" ref="C217:D217" si="52">IF($C$203="profit",C191,IF($C$203="fix",C91,C139))</f>
         <v>0</v>
       </c>
       <c r="D217" s="250">
@@ -9443,15 +9442,15 @@
         <v>17.476199999999999</v>
       </c>
       <c r="G217" s="172"/>
-      <c r="I217" s="260">
+      <c r="I217" s="259">
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
-      <c r="J217" s="260">
+      <c r="J217" s="259">
         <f t="shared" si="48"/>
         <v>16.643999999999998</v>
       </c>
-      <c r="K217" s="261">
+      <c r="K217" s="260">
         <f t="shared" si="49"/>
         <v>0.83220000000000027</v>
       </c>
@@ -9461,7 +9460,7 @@
         <v>109</v>
       </c>
       <c r="C218" s="250">
-        <f t="shared" ref="C218:F218" si="53">IF($C$203="profit",C192,IF($C$203="fix",C92,C140))</f>
+        <f t="shared" ref="C218:E218" si="53">IF($C$203="profit",C192,IF($C$203="fix",C92,C140))</f>
         <v>0</v>
       </c>
       <c r="D218" s="250">
@@ -9477,15 +9476,15 @@
         <v>14.891999999999999</v>
       </c>
       <c r="G218" s="172"/>
-      <c r="I218" s="260">
+      <c r="I218" s="259">
         <f t="shared" si="51"/>
         <v>0</v>
       </c>
-      <c r="J218" s="260">
+      <c r="J218" s="259">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="K218" s="260">
+      <c r="K218" s="259">
         <f t="shared" si="49"/>
         <v>14.891999999999999</v>
       </c>
@@ -10104,7 +10103,7 @@
       </c>
       <c r="C259" s="159">
         <f>C253+C209+C232</f>
-        <v>81.679000000000002</v>
+        <v>81.677459999999996</v>
       </c>
       <c r="D259" s="160">
         <f t="shared" ref="D259:F259" si="74">D253+D209+D232</f>
@@ -10208,11 +10207,11 @@
       </c>
       <c r="C265" s="159">
         <f>C259</f>
-        <v>81.679000000000002</v>
+        <v>81.677459999999996</v>
       </c>
       <c r="D265" s="160">
         <f>D259-C259</f>
-        <v>-0.27246999999998422</v>
+        <v>-0.27092999999997858</v>
       </c>
       <c r="E265" s="160">
         <f t="shared" ref="E265:F266" si="78">E259-D259</f>
@@ -10296,7 +10295,7 @@
       </c>
       <c r="C273" s="179">
         <f>C265</f>
-        <v>81.679000000000002</v>
+        <v>81.677459999999996</v>
       </c>
       <c r="D273" s="179">
         <f>D266</f>
@@ -10321,7 +10320,7 @@
       </c>
       <c r="D274" s="188">
         <f>SUM(D275:D278)</f>
-        <v>-0.27246999999998422</v>
+        <v>-0.27092999999997858</v>
       </c>
       <c r="E274" s="188">
         <f t="shared" ref="E274:F274" si="80">SUM(E275:E278)</f>
@@ -10339,7 +10338,7 @@
       <c r="C275" s="181"/>
       <c r="D275" s="186">
         <f>D265</f>
-        <v>-0.27246999999998422</v>
+        <v>-0.27092999999997858</v>
       </c>
       <c r="E275" s="186">
         <f t="shared" ref="E275:F275" si="81">E265</f>
@@ -10392,11 +10391,11 @@
       </c>
       <c r="C279" s="182">
         <f>C273+C274</f>
-        <v>81.679000000000002</v>
+        <v>81.677459999999996</v>
       </c>
       <c r="D279" s="182">
         <f>D273+D274</f>
-        <v>81.134060000000034</v>
+        <v>81.135600000000039</v>
       </c>
       <c r="E279" s="182">
         <f>E273+E274</f>

</xml_diff>